<commit_message>
add test case of modlue cache config
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-configure-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-configure-test-data.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0465D6D-A92A-4CC9-A603-33DF59A61F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="6432" yWindow="6468" windowWidth="21132" windowHeight="10716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="moduleCacheConfig" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,26 +24,86 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>test-id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>rspStatus</t>
+  </si>
+  <si>
+    <t>rspCode</t>
+  </si>
+  <si>
+    <t>rspMessage</t>
+  </si>
+  <si>
+    <t>jinzu-connector-configure-test-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get module cache config</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>moduleName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>data-layer-api-engine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operate success.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +111,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +414,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add cache-configure cache controller case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-connector-configure-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-connector-configure-test-data.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC7CB00-B1CD-4458-9064-E9A79580F924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE26FCA-170B-441E-99F8-769AD6BC1906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="660" windowWidth="21960" windowHeight="12408" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23600" yWindow="-12610" windowWidth="28800" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="moduleCacheConfig" sheetId="1" r:id="rId1"/>
     <sheet name="saveCacheConfig" sheetId="2" r:id="rId2"/>
     <sheet name="updateCacheConfig" sheetId="3" r:id="rId3"/>
     <sheet name="deleteCacheConfig" sheetId="4" r:id="rId4"/>
+    <sheet name="getAllCacheNames" sheetId="5" r:id="rId5"/>
+    <sheet name="getCacheKeyAndValue" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>test-id</t>
   </si>
@@ -142,6 +144,46 @@
   </si>
   <si>
     <t>entityDataCacheTest</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get allCacheNames</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataList</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinzu-connector-configure-cache-test1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>auth,connector,dataSource,engine,entity,mapper,plugin,rule,transaction,licenseConfigEncrypted</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cacheName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>entityName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Site</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jinzu-connector-configure-cache-test2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> mapper,check get cache key and value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mapper</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -213,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -221,6 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6123A7AF-B7BC-4C02-A160-650D88E9980E}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
@@ -776,4 +819,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F39FE7-88EC-43FB-87D3-43257DC6FAB2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="3" width="26.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA940480-A2EA-4AFA-AFF8-F9C923E0CC88}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>